<commit_message>
Funcional hasta donde detalles siempre sea una lista, faltaria mapear bien el tipo de dato de toda la estructura
</commit_message>
<xml_diff>
--- a/archivos_excel/factura.xlsx
+++ b/archivos_excel/factura.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AT-Redabierta\Documents\Local Repos\GoProcesadorExcel\archivos_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB3DB6A-8764-44A9-8DF6-8672E207BBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1442D9F9-C924-4FD4-B66A-0FE8755A93F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{76A9055E-E653-4319-A187-EA89127986D3}"/>
   </bookViews>
@@ -794,7 +794,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>